<commit_message>
updated the excel with all dates updated
</commit_message>
<xml_diff>
--- a/CS5110 - Project_Schedule_Timeline.xlsx
+++ b/CS5110 - Project_Schedule_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpatel\Desktop\Linkdin_Job_ANalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D6B85B-6A96-4816-AE17-1A444E337336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975838D1-431D-428B-97A3-F7774B4AA89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <t>Endpoint returns structured JSON</t>
   </si>
   <si>
-    <t>Streamlit/Plotly Dashboard (skills/region/salary)</t>
-  </si>
-  <si>
     <t>Top skills, locations &amp; salary distributions</t>
   </si>
   <si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>FastAPI endpoint for inference; React Frontend UI; Plotly dashboards (skills, salary, hotspots); demo dataset.</t>
+  </si>
+  <si>
+    <t>Dashboard (skills/region/salary)</t>
   </si>
 </sst>
 </file>
@@ -420,16 +420,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -826,9 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -931,7 +934,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>24</v>
@@ -947,15 +950,15 @@
         <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>24</v>
@@ -971,10 +974,10 @@
         <v>4</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -995,7 +998,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>94</v>
@@ -1019,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>96</v>
@@ -1027,7 +1030,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>16</v>
@@ -1043,10 +1046,10 @@
         <v>4</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1067,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>98</v>
@@ -1075,7 +1078,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>18</v>
@@ -1091,18 +1094,18 @@
         <v>7</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="C16" s="7">
         <v>45992</v>
@@ -1115,15 +1118,15 @@
         <v>5</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>18</v>
@@ -1139,15 +1142,15 @@
         <v>7</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>67</v>
@@ -1156,65 +1159,65 @@
         <v>45999</v>
       </c>
       <c r="D18" s="7">
-        <v>46003</v>
+        <v>45999</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="7">
-        <v>46001</v>
+        <v>45999</v>
       </c>
       <c r="D19" s="7">
-        <v>46004</v>
+        <v>45999</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>67</v>
       </c>
       <c r="C20" s="7">
-        <v>46005</v>
+        <v>45999</v>
       </c>
       <c r="D20" s="7">
-        <v>46005</v>
+        <v>45999</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1259,7 +1262,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1409,7 +1412,7 @@
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>

</xml_diff>